<commit_message>
updated mysql and oracle related changes
</commit_message>
<xml_diff>
--- a/output/P1.xlsx
+++ b/output/P1.xlsx
@@ -15,8 +15,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts>
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="1" formatCode="#,##0.00"/>
-    <numFmt numFmtId="2" formatCode="d-M-yyyy"/>
+    <numFmt numFmtId="1" formatCode="#,##0.############"/>
+    <numFmt numFmtId="2" formatCode="d-MMM-yyyy"/>
   </numFmts>
   <fonts>
     <font>
@@ -68,7 +68,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="CEDE1F"/>
+        <fgColor rgb="FFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -76,7 +76,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="CEDE1F"/>
+        <fgColor rgb="0000FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -178,7 +178,7 @@
       <c r="A1" s="1" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">Product Header</t>
+            <t xml:space="preserve">PRODUCT REPORT</t>
           </r>
         </is>
       </c>
@@ -225,8 +225,12 @@
       </c>
     </row>
     <row r="3" customHeight="1" ht="15">
-      <c r="A3" s="4" t="n">
-        <v>10.0</v>
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">10</t>
+          </r>
+        </is>
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
@@ -236,10 +240,10 @@
         </is>
       </c>
       <c r="C3" s="5" t="n">
-        <v>1.29899004166144E15</v>
+        <v>10000.23</v>
       </c>
       <c r="D3" s="6">
-        <v>43780.0</v>
+        <v>43779.95833333349</v>
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
@@ -250,8 +254,12 @@
       </c>
     </row>
     <row r="4" customHeight="1" ht="15">
-      <c r="A4" s="4" t="n">
-        <v>10.0</v>
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">10</t>
+          </r>
+        </is>
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
@@ -261,10 +269,10 @@
         </is>
       </c>
       <c r="C4" s="5" t="n">
-        <v>3.43298984116224E14</v>
+        <v>10000.23</v>
       </c>
       <c r="D4" s="6">
-        <v>27759.0</v>
+        <v>27758.95833333349</v>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
@@ -275,8 +283,12 @@
       </c>
     </row>
     <row r="5" customHeight="1" ht="15">
-      <c r="A5" s="4" t="n">
-        <v>10.0</v>
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">10</t>
+          </r>
+        </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
@@ -286,10 +298,10 @@
         </is>
       </c>
       <c r="C5" s="5" t="n">
-        <v>3.43298984116224E14</v>
+        <v>10000.23</v>
       </c>
       <c r="D5" s="6">
-        <v>27759.0</v>
+        <v>27758.95833333349</v>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>

</xml_diff>